<commit_message>
seed of municipalities in progress
</commit_message>
<xml_diff>
--- a/lib/seeds/municipalities/Lista2.xlsx
+++ b/lib/seeds/municipalities/Lista2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2de5b8db183ef9c/Documents/CA/EACE/controle/Planilhas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{A189221F-1845-4171-8CC8-DD46E71CE2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C12B6780-85D2-4089-A3D6-A6D60E385F7A}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{A189221F-1845-4171-8CC8-DD46E71CE2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD198F64-BCB4-4A3F-A343-17EC2EF1E69E}"/>
   <bookViews>
-    <workbookView xWindow="-28035" yWindow="645" windowWidth="27180" windowHeight="14760" tabRatio="776" xr2:uid="{BFD4F44D-72C7-4C72-BDE1-AEE890295311}"/>
+    <workbookView xWindow="-27360" yWindow="1530" windowWidth="27180" windowHeight="13290" tabRatio="776" xr2:uid="{BFD4F44D-72C7-4C72-BDE1-AEE890295311}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista2-96" sheetId="5" r:id="rId1"/>
@@ -1202,15 +1202,6 @@
     <t>(86) 3331-0059</t>
   </si>
   <si>
-    <t>municipality-name</t>
-  </si>
-  <si>
-    <t>original-coordinator</t>
-  </si>
-  <si>
-    <t>current-coordinator</t>
-  </si>
-  <si>
     <t>contact-name</t>
   </si>
   <si>
@@ -1233,6 +1224,15 @@
   </si>
   <si>
     <t>date-memo-sent</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>coord-ori</t>
+  </si>
+  <si>
+    <t>corrd-current</t>
   </si>
 </sst>
 </file>
@@ -1385,7 +1385,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1445,8 +1445,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1779,7 +1778,7 @@
   <dimension ref="A1:L98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1789,7 +1788,7 @@
     <col min="5" max="5" width="38.88671875" customWidth="1"/>
     <col min="6" max="6" width="36.21875" customWidth="1"/>
     <col min="7" max="7" width="32.21875" customWidth="1"/>
-    <col min="8" max="8" width="42.33203125" style="21" customWidth="1"/>
+    <col min="8" max="8" width="42.33203125" customWidth="1"/>
     <col min="9" max="9" width="18.44140625" customWidth="1"/>
     <col min="10" max="10" width="16.6640625" customWidth="1"/>
     <col min="11" max="11" width="14.88671875" customWidth="1"/>
@@ -1801,37 +1800,37 @@
         <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D1" t="s">
+        <v>398</v>
+      </c>
+      <c r="E1" t="s">
         <v>388</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>389</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>390</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>391</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>392</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>393</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="K1" t="s">
         <v>394</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>395</v>
-      </c>
-      <c r="J1" t="s">
-        <v>396</v>
-      </c>
-      <c r="K1" t="s">
-        <v>397</v>
-      </c>
-      <c r="L1" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1868,7 +1867,7 @@
       <c r="K2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L2" s="26">
+      <c r="L2" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -1906,7 +1905,7 @@
       <c r="K3" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L3" s="26">
+      <c r="L3" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -1944,7 +1943,7 @@
       <c r="K4" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L4" s="26">
+      <c r="L4" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -1982,7 +1981,7 @@
       <c r="K5" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L5" s="26">
+      <c r="L5" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2020,7 +2019,7 @@
       <c r="K6" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L6" s="26">
+      <c r="L6" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2056,7 +2055,7 @@
       <c r="K7" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L7" s="26">
+      <c r="L7" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2094,7 +2093,7 @@
       <c r="K8" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L8" s="26">
+      <c r="L8" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2132,7 +2131,7 @@
       <c r="K9" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L9" s="26">
+      <c r="L9" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2170,7 +2169,7 @@
       <c r="K10" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L10" s="26">
+      <c r="L10" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2208,7 +2207,7 @@
       <c r="K11" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L11" s="26">
+      <c r="L11" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2246,7 +2245,7 @@
       <c r="K12" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="L12" s="26">
+      <c r="L12" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2284,7 +2283,7 @@
       <c r="K13" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L13" s="26">
+      <c r="L13" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2358,7 +2357,7 @@
       <c r="K15" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L15" s="26">
+      <c r="L15" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2396,7 +2395,7 @@
       <c r="K16" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L16" s="26">
+      <c r="L16" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2434,7 +2433,7 @@
       <c r="K17" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L17" s="26">
+      <c r="L17" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2472,7 +2471,7 @@
       <c r="K18" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L18" s="26">
+      <c r="L18" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2510,7 +2509,7 @@
       <c r="K19" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L19" s="26">
+      <c r="L19" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2548,7 +2547,7 @@
       <c r="K20" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L20" s="26">
+      <c r="L20" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2586,7 +2585,7 @@
       <c r="K21" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L21" s="26">
+      <c r="L21" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2624,7 +2623,7 @@
       <c r="K22" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="L22" s="26">
+      <c r="L22" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2662,7 +2661,7 @@
       <c r="K23" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="L23" s="26">
+      <c r="L23" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2700,7 +2699,7 @@
       <c r="K24" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L24" s="26">
+      <c r="L24" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2738,7 +2737,7 @@
       <c r="K25" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L25" s="26">
+      <c r="L25" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2776,7 +2775,7 @@
       <c r="K26" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L26" s="26">
+      <c r="L26" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2814,7 +2813,7 @@
       <c r="K27" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L27" s="26">
+      <c r="L27" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2852,7 +2851,7 @@
       <c r="K28" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L28" s="26">
+      <c r="L28" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2890,7 +2889,7 @@
       <c r="K29" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L29" s="26">
+      <c r="L29" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2928,7 +2927,7 @@
       <c r="K30" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L30" s="26">
+      <c r="L30" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -2966,7 +2965,7 @@
       <c r="K31" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="L31" s="26">
+      <c r="L31" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3004,7 +3003,7 @@
       <c r="K32" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L32" s="26">
+      <c r="L32" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3042,7 +3041,7 @@
       <c r="K33" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L33" s="26">
+      <c r="L33" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3080,7 +3079,7 @@
       <c r="K34" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L34" s="26">
+      <c r="L34" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3118,7 +3117,7 @@
       <c r="K35" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L35" s="26">
+      <c r="L35" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3144,7 +3143,7 @@
       <c r="G36" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="H36" s="21" t="s">
+      <c r="H36" t="s">
         <v>221</v>
       </c>
       <c r="I36" s="6">
@@ -3156,7 +3155,7 @@
       <c r="K36" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L36" s="26">
+      <c r="L36" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3194,7 +3193,7 @@
       <c r="K37" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L37" s="26">
+      <c r="L37" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3220,7 +3219,7 @@
       <c r="G38" s="20" t="s">
         <v>368</v>
       </c>
-      <c r="H38" s="22" t="s">
+      <c r="H38" s="21" t="s">
         <v>228</v>
       </c>
       <c r="I38" s="6">
@@ -3232,7 +3231,7 @@
       <c r="K38" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L38" s="26">
+      <c r="L38" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3270,7 +3269,7 @@
       <c r="K39" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L39" s="26">
+      <c r="L39" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3308,7 +3307,7 @@
       <c r="K40" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L40" s="26">
+      <c r="L40" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3334,7 +3333,7 @@
       <c r="G41" s="20" t="s">
         <v>371</v>
       </c>
-      <c r="H41" s="23" t="s">
+      <c r="H41" s="22" t="s">
         <v>236</v>
       </c>
       <c r="I41" s="6">
@@ -3346,7 +3345,7 @@
       <c r="K41" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L41" s="26">
+      <c r="L41" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3384,7 +3383,7 @@
       <c r="K42" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L42" s="26">
+      <c r="L42" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3422,7 +3421,7 @@
       <c r="K43" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L43" s="26">
+      <c r="L43" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3460,7 +3459,7 @@
       <c r="K44" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L44" s="26">
+      <c r="L44" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3498,7 +3497,7 @@
       <c r="K45" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L45" s="26">
+      <c r="L45" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3536,7 +3535,7 @@
       <c r="K46" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L46" s="26">
+      <c r="L46" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3574,7 +3573,7 @@
       <c r="K47" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L47" s="26">
+      <c r="L47" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3612,7 +3611,7 @@
       <c r="K48" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L48" s="26">
+      <c r="L48" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3650,7 +3649,7 @@
       <c r="K49" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L49" s="26">
+      <c r="L49" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3688,7 +3687,7 @@
       <c r="K50" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L50" s="26">
+      <c r="L50" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3726,7 +3725,7 @@
       <c r="K51" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L51" s="26">
+      <c r="L51" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3764,7 +3763,7 @@
       <c r="K52" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L52" s="26">
+      <c r="L52" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3802,7 +3801,7 @@
       <c r="K53" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L53" s="26">
+      <c r="L53" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3840,7 +3839,7 @@
       <c r="K54" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L54" s="26">
+      <c r="L54" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3878,7 +3877,7 @@
       <c r="K55" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L55" s="26">
+      <c r="L55" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -3916,7 +3915,7 @@
       <c r="K56" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L56" s="26">
+      <c r="L56" s="25">
         <v>45579</v>
       </c>
     </row>
@@ -3954,7 +3953,7 @@
       <c r="K57" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L57" s="26">
+      <c r="L57" s="25">
         <v>45579</v>
       </c>
     </row>
@@ -3992,7 +3991,7 @@
       <c r="K58" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L58" s="26">
+      <c r="L58" s="25">
         <v>45579</v>
       </c>
     </row>
@@ -4030,7 +4029,7 @@
       <c r="K59" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L59" s="26">
+      <c r="L59" s="25">
         <v>45579</v>
       </c>
     </row>
@@ -4056,7 +4055,7 @@
       <c r="G60" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="H60" s="24" t="s">
+      <c r="H60" s="23" t="s">
         <v>384</v>
       </c>
       <c r="I60" s="6">
@@ -4068,7 +4067,7 @@
       <c r="K60" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L60" s="26">
+      <c r="L60" s="25">
         <v>45579</v>
       </c>
     </row>
@@ -4106,7 +4105,7 @@
       <c r="K61" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L61" s="26">
+      <c r="L61" s="25">
         <v>45579</v>
       </c>
     </row>
@@ -4144,7 +4143,7 @@
       <c r="K62" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L62" s="26">
+      <c r="L62" s="25">
         <v>45579</v>
       </c>
     </row>
@@ -4182,7 +4181,7 @@
       <c r="K63" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L63" s="26">
+      <c r="L63" s="25">
         <v>45579</v>
       </c>
     </row>
@@ -4220,7 +4219,7 @@
       <c r="K64" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L64" s="26">
+      <c r="L64" s="25">
         <v>45579</v>
       </c>
     </row>
@@ -4258,7 +4257,7 @@
       <c r="K65" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L65" s="26">
+      <c r="L65" s="25">
         <v>45579</v>
       </c>
     </row>
@@ -4296,7 +4295,7 @@
       <c r="K66" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L66" s="26">
+      <c r="L66" s="25">
         <v>45579</v>
       </c>
     </row>
@@ -4334,7 +4333,7 @@
       <c r="K67" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L67" s="26">
+      <c r="L67" s="25">
         <v>45579</v>
       </c>
     </row>
@@ -4426,7 +4425,7 @@
       <c r="G71" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="H71" s="25" t="s">
+      <c r="H71" s="24" t="s">
         <v>385</v>
       </c>
       <c r="I71" s="6">
@@ -4438,7 +4437,7 @@
       <c r="K71" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L71" s="26">
+      <c r="L71" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -4472,7 +4471,7 @@
       <c r="K72" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L72" s="26">
+      <c r="L72" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -4506,7 +4505,7 @@
       <c r="K73" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L73" s="26">
+      <c r="L73" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -4540,7 +4539,7 @@
       <c r="K74" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L74" s="26">
+      <c r="L74" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -4640,7 +4639,7 @@
       <c r="K78" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L78" s="26">
+      <c r="L78" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -4704,7 +4703,7 @@
       <c r="K80" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L80" s="26">
+      <c r="L80" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -4738,7 +4737,7 @@
       <c r="K81" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L81" s="26">
+      <c r="L81" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -4776,7 +4775,7 @@
       <c r="K82" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L82" s="26">
+      <c r="L82" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -4832,7 +4831,7 @@
       <c r="K84" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L84" s="26">
+      <c r="L84" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -4888,7 +4887,7 @@
       <c r="K86" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L86" s="26">
+      <c r="L86" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -4922,7 +4921,7 @@
       <c r="K87" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L87" s="26">
+      <c r="L87" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -5004,7 +5003,7 @@
       <c r="K90" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L90" s="26">
+      <c r="L90" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -5038,7 +5037,7 @@
       <c r="K91" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L91" s="26">
+      <c r="L91" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -5072,7 +5071,7 @@
       <c r="K92" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L92" s="26">
+      <c r="L92" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -5106,7 +5105,7 @@
       <c r="K93" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L93" s="26">
+      <c r="L93" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -5140,7 +5139,7 @@
       <c r="K94" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L94" s="26">
+      <c r="L94" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -5174,7 +5173,7 @@
       <c r="K95" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L95" s="26">
+      <c r="L95" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -5208,7 +5207,7 @@
       <c r="K96" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="L96" s="26">
+      <c r="L96" s="25">
         <v>45566</v>
       </c>
     </row>
@@ -5246,7 +5245,7 @@
       <c r="K97" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L97" s="26">
+      <c r="L97" s="25">
         <v>45566</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refazendo o seed de municipios
</commit_message>
<xml_diff>
--- a/lib/seeds/municipalities/Lista2.xlsx
+++ b/lib/seeds/municipalities/Lista2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2de5b8db183ef9c/Documents/CA/EACE/controle/Planilhas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{A189221F-1845-4171-8CC8-DD46E71CE2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD198F64-BCB4-4A3F-A343-17EC2EF1E69E}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{7C52FCFD-1B31-4900-8521-B506C2563E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6813C139-E805-41F0-B282-FF22ED7A58BD}"/>
   <bookViews>
-    <workbookView xWindow="-27360" yWindow="1530" windowWidth="27180" windowHeight="13290" tabRatio="776" xr2:uid="{BFD4F44D-72C7-4C72-BDE1-AEE890295311}"/>
+    <workbookView xWindow="-26595" yWindow="1050" windowWidth="26100" windowHeight="14190" tabRatio="776" xr2:uid="{BFD4F44D-72C7-4C72-BDE1-AEE890295311}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista2-96" sheetId="5" r:id="rId1"/>
@@ -1214,9 +1214,6 @@
     <t>contact-email</t>
   </si>
   <si>
-    <t>numer-of-attempts</t>
-  </si>
-  <si>
     <t>date-last-attempt</t>
   </si>
   <si>
@@ -1232,7 +1229,10 @@
     <t>coord-ori</t>
   </si>
   <si>
-    <t>corrd-current</t>
+    <t>coord-current</t>
+  </si>
+  <si>
+    <t>number-of-attempts</t>
   </si>
 </sst>
 </file>
@@ -1242,7 +1242,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1321,6 +1321,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1385,7 +1392,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1458,6 +1465,7 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hiperlink" xfId="3" builtinId="8"/>
@@ -1777,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ADFCF75-0275-4480-9278-B53509A2BDD1}">
   <dimension ref="A1:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1800,13 +1808,13 @@
         <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C1" t="s">
         <v>396</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>397</v>
-      </c>
-      <c r="D1" t="s">
-        <v>398</v>
       </c>
       <c r="E1" t="s">
         <v>388</v>
@@ -1821,16 +1829,16 @@
         <v>391</v>
       </c>
       <c r="I1" t="s">
+        <v>398</v>
+      </c>
+      <c r="J1" t="s">
         <v>392</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>393</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>394</v>
-      </c>
-      <c r="L1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2177,7 +2185,7 @@
       <c r="A11" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="26" t="s">
         <v>86</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -5250,9 +5258,7 @@
       </c>
     </row>
     <row r="98" spans="1:12">
-      <c r="B98" s="1">
-        <v>96</v>
-      </c>
+      <c r="B98" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B98">

</xml_diff>

<commit_message>
parei no problema da data
</commit_message>
<xml_diff>
--- a/lib/seeds/municipalities/Lista2.xlsx
+++ b/lib/seeds/municipalities/Lista2.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2de5b8db183ef9c/Documents/CA/EACE/controle/Planilhas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{7C52FCFD-1B31-4900-8521-B506C2563E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6813C139-E805-41F0-B282-FF22ED7A58BD}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{7C52FCFD-1B31-4900-8521-B506C2563E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCCC8E7B-E118-4781-8FB8-861ADD70DA07}"/>
   <bookViews>
-    <workbookView xWindow="-26595" yWindow="1050" windowWidth="26100" windowHeight="14190" tabRatio="776" xr2:uid="{BFD4F44D-72C7-4C72-BDE1-AEE890295311}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" tabRatio="776" xr2:uid="{BFD4F44D-72C7-4C72-BDE1-AEE890295311}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista2-96" sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="398">
   <si>
     <t>PI</t>
   </si>
@@ -417,9 +418,6 @@
   </si>
   <si>
     <t>gabinetepmtv@gmail.com</t>
-  </si>
-  <si>
-    <t>115/10</t>
   </si>
   <si>
     <t>Mauricio de Vasconcelos</t>
@@ -1239,9 +1237,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d/m"/>
-  </numFmts>
   <fonts count="13">
     <font>
       <sz val="11"/>
@@ -1392,7 +1387,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1412,9 +1407,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1785,22 +1777,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ADFCF75-0275-4480-9278-B53509A2BDD1}">
   <dimension ref="A1:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J88" sqref="J88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
-    <col min="3" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="38.88671875" customWidth="1"/>
-    <col min="6" max="6" width="36.21875" customWidth="1"/>
-    <col min="7" max="7" width="32.21875" customWidth="1"/>
-    <col min="8" max="8" width="42.33203125" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" customWidth="1"/>
+    <col min="8" max="8" width="42.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1808,37 +1800,37 @@
         <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C1" t="s">
         <v>395</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>396</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>387</v>
+      </c>
+      <c r="F1" t="s">
+        <v>388</v>
+      </c>
+      <c r="G1" t="s">
+        <v>389</v>
+      </c>
+      <c r="H1" t="s">
+        <v>390</v>
+      </c>
+      <c r="I1" t="s">
         <v>397</v>
       </c>
-      <c r="E1" t="s">
-        <v>388</v>
-      </c>
-      <c r="F1" t="s">
-        <v>389</v>
-      </c>
-      <c r="G1" t="s">
-        <v>390</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>391</v>
       </c>
-      <c r="I1" t="s">
-        <v>398</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>392</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>393</v>
-      </c>
-      <c r="L1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1869,13 +1861,13 @@
       <c r="I2" s="6">
         <v>2</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="24">
         <v>45579</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -1907,13 +1899,13 @@
       <c r="I3" s="6">
         <v>1</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="24">
         <v>45580</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L3" s="25">
+      <c r="L3" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -1936,8 +1928,8 @@
       <c r="F4" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>386</v>
+      <c r="G4" s="8" t="s">
+        <v>385</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>113</v>
@@ -1945,13 +1937,13 @@
       <c r="I4" s="6">
         <v>2</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="24">
         <v>45580</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -1974,7 +1966,7 @@
       <c r="F5" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>115</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -1983,13 +1975,13 @@
       <c r="I5" s="6">
         <v>1</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="24">
         <v>45580</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2012,22 +2004,22 @@
       <c r="F6" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>120</v>
       </c>
       <c r="I6" s="6">
         <v>3</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="24">
         <v>45580</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L6" s="25">
+      <c r="L6" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2050,20 +2042,20 @@
       <c r="F7" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>122</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="6">
         <v>3</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="24">
         <v>45580</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2086,7 +2078,7 @@
       <c r="F8" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>125</v>
       </c>
       <c r="H8" s="4" t="s">
@@ -2095,13 +2087,13 @@
       <c r="I8" s="6">
         <v>2</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>127</v>
+      <c r="J8" s="24">
+        <v>45580</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L8" s="25">
+      <c r="L8" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2119,27 +2111,27 @@
         <v>101</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="I9" s="6">
         <v>1</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="24">
         <v>45580</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2157,27 +2149,27 @@
         <v>101</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="I10" s="6">
         <v>2</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="24">
         <v>45579</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L10" s="25">
+      <c r="L10" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2185,7 +2177,7 @@
       <c r="A11" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>86</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -2195,27 +2187,27 @@
         <v>101</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="G11" s="9" t="s">
+      <c r="H11" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>137</v>
       </c>
       <c r="I11" s="6">
         <v>2</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="24">
         <v>45580</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L11" s="25">
+      <c r="L11" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2233,27 +2225,27 @@
         <v>101</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="I12" s="6">
         <v>2</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="24">
         <v>45579</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="L12" s="25">
+      <c r="L12" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2271,27 +2263,27 @@
         <v>101</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="H13" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="I13" s="6">
         <v>2</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="24">
         <v>45580</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2309,21 +2301,21 @@
         <v>101</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="I14" s="6">
         <v>3</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="24">
         <v>45580</v>
       </c>
       <c r="K14" s="6" t="s">
@@ -2345,27 +2337,27 @@
         <v>101</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G15" s="9" t="s">
+      <c r="H15" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="I15" s="6">
         <v>3</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="24">
         <v>45580</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L15" s="25">
+      <c r="L15" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2383,27 +2375,27 @@
         <v>101</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="H16" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>155</v>
       </c>
       <c r="I16" s="6">
         <v>2</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="24">
         <v>45580</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L16" s="25">
+      <c r="L16" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2421,27 +2413,27 @@
         <v>101</v>
       </c>
       <c r="E17" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="G17" s="9" t="s">
+      <c r="H17" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>158</v>
       </c>
       <c r="I17" s="6">
         <v>2</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="24">
         <v>45580</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2459,27 +2451,27 @@
         <v>101</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="G18" s="9" t="s">
+      <c r="H18" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>161</v>
       </c>
       <c r="I18" s="6">
         <v>2</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J18" s="24">
         <v>45579</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L18" s="25">
+      <c r="L18" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2497,27 +2489,27 @@
         <v>101</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G19" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="H19" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>165</v>
       </c>
       <c r="I19" s="6">
         <v>3</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19" s="24">
         <v>45580</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L19" s="25">
+      <c r="L19" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2535,27 +2527,27 @@
         <v>101</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G20" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G20" s="9" t="s">
+      <c r="H20" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>168</v>
       </c>
       <c r="I20" s="6">
         <v>2</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="24">
         <v>45580</v>
       </c>
       <c r="K20" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L20" s="25">
+      <c r="L20" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2573,27 +2565,27 @@
         <v>101</v>
       </c>
       <c r="E21" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="G21" s="6" t="s">
+      <c r="H21" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="I21" s="6">
         <v>2</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J21" s="24">
         <v>45580</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L21" s="25">
+      <c r="L21" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2611,27 +2603,27 @@
         <v>101</v>
       </c>
       <c r="E22" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="G22" s="6" t="s">
+      <c r="H22" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="I22" s="6">
         <v>1</v>
       </c>
-      <c r="J22" s="8">
+      <c r="J22" s="24">
         <v>45580</v>
       </c>
       <c r="K22" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="L22" s="25">
+      <c r="L22" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2649,27 +2641,27 @@
         <v>101</v>
       </c>
       <c r="E23" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>366</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>175</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>367</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>176</v>
       </c>
       <c r="I23" s="6">
         <v>1</v>
       </c>
-      <c r="J23" s="8">
+      <c r="J23" s="24">
         <v>45574</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="L23" s="25">
+      <c r="L23" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2687,27 +2679,27 @@
         <v>101</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>124</v>
       </c>
       <c r="G24" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="H24" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="I24" s="6">
         <v>1</v>
       </c>
-      <c r="J24" s="8">
+      <c r="J24" s="24">
         <v>45580</v>
       </c>
       <c r="K24" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L24" s="25">
+      <c r="L24" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2725,27 +2717,27 @@
         <v>101</v>
       </c>
       <c r="E25" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="G25" s="6" t="s">
+      <c r="H25" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="I25" s="6">
         <v>2</v>
       </c>
-      <c r="J25" s="8">
+      <c r="J25" s="24">
         <v>45580</v>
       </c>
       <c r="K25" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L25" s="25">
+      <c r="L25" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2763,27 +2755,27 @@
         <v>101</v>
       </c>
       <c r="E26" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="H26" s="5" t="s">
         <v>185</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>186</v>
       </c>
       <c r="I26" s="6">
         <v>1</v>
       </c>
-      <c r="J26" s="8">
+      <c r="J26" s="24">
         <v>45580</v>
       </c>
       <c r="K26" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L26" s="25">
+      <c r="L26" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2801,27 +2793,27 @@
         <v>101</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>118</v>
       </c>
       <c r="G27" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H27" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="I27" s="6">
         <v>2</v>
       </c>
-      <c r="J27" s="8">
+      <c r="J27" s="24">
         <v>45580</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L27" s="25">
+      <c r="L27" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2839,27 +2831,27 @@
         <v>101</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>118</v>
       </c>
       <c r="G28" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="I28" s="6">
         <v>1</v>
       </c>
-      <c r="J28" s="8">
+      <c r="J28" s="24">
         <v>45580</v>
       </c>
       <c r="K28" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L28" s="25">
+      <c r="L28" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2877,27 +2869,27 @@
         <v>101</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>118</v>
       </c>
       <c r="G29" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>195</v>
       </c>
       <c r="I29" s="6">
         <v>2</v>
       </c>
-      <c r="J29" s="8">
+      <c r="J29" s="24">
         <v>45580</v>
       </c>
       <c r="K29" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L29" s="25">
+      <c r="L29" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2915,27 +2907,27 @@
         <v>101</v>
       </c>
       <c r="E30" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="H30" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>199</v>
       </c>
       <c r="I30" s="6">
         <v>2</v>
       </c>
-      <c r="J30" s="8">
+      <c r="J30" s="24">
         <v>45580</v>
       </c>
       <c r="K30" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L30" s="25">
+      <c r="L30" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2953,27 +2945,27 @@
         <v>101</v>
       </c>
       <c r="E31" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G31" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="G31" s="6" t="s">
+      <c r="H31" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>202</v>
       </c>
       <c r="I31" s="6">
         <v>1</v>
       </c>
-      <c r="J31" s="8">
+      <c r="J31" s="24">
         <v>45574</v>
       </c>
       <c r="K31" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="L31" s="25">
+      <c r="L31" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -2991,27 +2983,27 @@
         <v>101</v>
       </c>
       <c r="E32" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="G32" s="6" t="s">
+      <c r="H32" s="5" t="s">
         <v>204</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>205</v>
       </c>
       <c r="I32" s="6">
         <v>2</v>
       </c>
-      <c r="J32" s="8">
+      <c r="J32" s="24">
         <v>45580</v>
       </c>
       <c r="K32" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L32" s="25">
+      <c r="L32" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3029,27 +3021,27 @@
         <v>101</v>
       </c>
       <c r="E33" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="H33" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>209</v>
       </c>
       <c r="I33" s="6">
         <v>3</v>
       </c>
-      <c r="J33" s="8">
+      <c r="J33" s="24">
         <v>45580</v>
       </c>
       <c r="K33" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L33" s="25">
+      <c r="L33" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3067,27 +3059,27 @@
         <v>101</v>
       </c>
       <c r="E34" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="G34" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="H34" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>213</v>
       </c>
       <c r="I34" s="6">
         <v>2</v>
       </c>
-      <c r="J34" s="8">
+      <c r="J34" s="24">
         <v>45579</v>
       </c>
       <c r="K34" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L34" s="25">
+      <c r="L34" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3105,27 +3097,27 @@
         <v>101</v>
       </c>
       <c r="E35" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="G35" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="H35" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>217</v>
       </c>
       <c r="I35" s="6">
         <v>2</v>
       </c>
-      <c r="J35" s="8">
+      <c r="J35" s="24">
         <v>45579</v>
       </c>
       <c r="K35" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L35" s="25">
+      <c r="L35" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3143,27 +3135,27 @@
         <v>101</v>
       </c>
       <c r="E36" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="G36" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="H36" t="s">
         <v>220</v>
-      </c>
-      <c r="H36" t="s">
-        <v>221</v>
       </c>
       <c r="I36" s="6">
         <v>1</v>
       </c>
-      <c r="J36" s="8">
+      <c r="J36" s="24">
         <v>45580</v>
       </c>
       <c r="K36" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L36" s="25">
+      <c r="L36" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3181,27 +3173,27 @@
         <v>101</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>118</v>
       </c>
       <c r="G37" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="H37" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="I37" s="6">
         <v>1</v>
       </c>
-      <c r="J37" s="8">
+      <c r="J37" s="24">
         <v>45580</v>
       </c>
       <c r="K37" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L37" s="25">
+      <c r="L37" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3213,33 +3205,33 @@
         <v>51</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E38" s="5" t="s">
+      <c r="F38" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="G38" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="H38" s="20" t="s">
         <v>227</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>368</v>
-      </c>
-      <c r="H38" s="21" t="s">
-        <v>228</v>
       </c>
       <c r="I38" s="6">
         <v>3</v>
       </c>
-      <c r="J38" s="8">
+      <c r="J38" s="24">
         <v>45569</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L38" s="25">
+        <v>228</v>
+      </c>
+      <c r="L38" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3251,33 +3243,33 @@
         <v>47</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>231</v>
+        <v>224</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>230</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="G39" s="20" t="s">
-        <v>369</v>
-      </c>
-      <c r="H39" s="12" t="s">
-        <v>232</v>
+      <c r="G39" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>231</v>
       </c>
       <c r="I39" s="6">
         <v>4</v>
       </c>
-      <c r="J39" s="8">
+      <c r="J39" s="24">
         <v>45569</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L39" s="25">
+        <v>228</v>
+      </c>
+      <c r="L39" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3289,33 +3281,33 @@
         <v>65</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="G40" s="20" t="s">
-        <v>370</v>
+      <c r="G40" s="19" t="s">
+        <v>369</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I40" s="6">
         <v>4</v>
       </c>
-      <c r="J40" s="8">
+      <c r="J40" s="24">
         <v>45569</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L40" s="25">
+        <v>228</v>
+      </c>
+      <c r="L40" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3327,33 +3319,33 @@
         <v>49</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>235</v>
+        <v>224</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>234</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="G41" s="20" t="s">
-        <v>371</v>
-      </c>
-      <c r="H41" s="22" t="s">
-        <v>236</v>
+      <c r="G41" s="19" t="s">
+        <v>370</v>
+      </c>
+      <c r="H41" s="21" t="s">
+        <v>235</v>
       </c>
       <c r="I41" s="6">
         <v>6</v>
       </c>
-      <c r="J41" s="8">
+      <c r="J41" s="24">
         <v>45569</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L41" s="25">
+        <v>228</v>
+      </c>
+      <c r="L41" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3365,33 +3357,33 @@
         <v>78</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E42" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="H42" s="5" t="s">
         <v>237</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G42" s="20" t="s">
-        <v>372</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>238</v>
       </c>
       <c r="I42" s="6">
         <v>10</v>
       </c>
-      <c r="J42" s="8">
+      <c r="J42" s="24">
         <v>45576</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L42" s="25">
+        <v>228</v>
+      </c>
+      <c r="L42" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3403,33 +3395,33 @@
         <v>48</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E43" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>372</v>
+      </c>
+      <c r="H43" s="13" t="s">
         <v>239</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>373</v>
-      </c>
-      <c r="H43" s="14" t="s">
-        <v>240</v>
       </c>
       <c r="I43" s="6">
         <v>6</v>
       </c>
-      <c r="J43" s="8">
+      <c r="J43" s="24">
         <v>45576</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L43" s="25">
+        <v>228</v>
+      </c>
+      <c r="L43" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3441,33 +3433,33 @@
         <v>54</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E44" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="G44" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="H44" s="13" t="s">
         <v>241</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G44" s="20" t="s">
-        <v>374</v>
-      </c>
-      <c r="H44" s="14" t="s">
-        <v>242</v>
       </c>
       <c r="I44" s="6">
         <v>4</v>
       </c>
-      <c r="J44" s="8">
+      <c r="J44" s="24">
         <v>45576</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L44" s="25">
+        <v>228</v>
+      </c>
+      <c r="L44" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3479,33 +3471,33 @@
         <v>75</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E45" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G45" s="19" t="s">
+        <v>374</v>
+      </c>
+      <c r="H45" s="13" t="s">
         <v>243</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="G45" s="20" t="s">
-        <v>375</v>
-      </c>
-      <c r="H45" s="14" t="s">
-        <v>244</v>
       </c>
       <c r="I45" s="6">
         <v>4</v>
       </c>
-      <c r="J45" s="8">
+      <c r="J45" s="24">
         <v>45580</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L45" s="25">
+        <v>228</v>
+      </c>
+      <c r="L45" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3517,33 +3509,33 @@
         <v>61</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E46" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="G46" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="F46" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G46" s="6" t="s">
+      <c r="H46" s="13" t="s">
         <v>246</v>
-      </c>
-      <c r="H46" s="14" t="s">
-        <v>247</v>
       </c>
       <c r="I46" s="6">
         <v>2</v>
       </c>
-      <c r="J46" s="8">
+      <c r="J46" s="24">
         <v>45580</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L46" s="25">
+        <v>228</v>
+      </c>
+      <c r="L46" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3555,33 +3547,33 @@
         <v>69</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E47" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G47" s="19" t="s">
+        <v>375</v>
+      </c>
+      <c r="H47" s="13" t="s">
         <v>248</v>
-      </c>
-      <c r="F47" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="G47" s="20" t="s">
-        <v>376</v>
-      </c>
-      <c r="H47" s="14" t="s">
-        <v>249</v>
       </c>
       <c r="I47" s="6">
         <v>3</v>
       </c>
-      <c r="J47" s="8">
+      <c r="J47" s="24">
         <v>45580</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L47" s="25">
+        <v>228</v>
+      </c>
+      <c r="L47" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3593,33 +3585,33 @@
         <v>73</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E48" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="H48" s="13" t="s">
         <v>250</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>251</v>
       </c>
       <c r="I48" s="6">
         <v>5</v>
       </c>
-      <c r="J48" s="8">
+      <c r="J48" s="24">
         <v>45580</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L48" s="25">
+        <v>228</v>
+      </c>
+      <c r="L48" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3631,33 +3623,33 @@
         <v>70</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E49" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="G49" s="19" t="s">
+        <v>377</v>
+      </c>
+      <c r="H49" s="13" t="s">
         <v>252</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G49" s="20" t="s">
-        <v>378</v>
-      </c>
-      <c r="H49" s="14" t="s">
-        <v>253</v>
       </c>
       <c r="I49" s="6">
         <v>3</v>
       </c>
-      <c r="J49" s="8">
+      <c r="J49" s="24">
         <v>45580</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L49" s="25">
+        <v>228</v>
+      </c>
+      <c r="L49" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3669,33 +3661,33 @@
         <v>53</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E50" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="F50" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="G50" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="H50" s="13" t="s">
         <v>254</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G50" s="20" t="s">
-        <v>379</v>
-      </c>
-      <c r="H50" s="14" t="s">
-        <v>255</v>
       </c>
       <c r="I50" s="6">
         <v>2</v>
       </c>
-      <c r="J50" s="8">
+      <c r="J50" s="24">
         <v>45580</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L50" s="25">
+        <v>228</v>
+      </c>
+      <c r="L50" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3707,33 +3699,33 @@
         <v>66</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E51" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="H51" s="13" t="s">
         <v>256</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="H51" s="14" t="s">
-        <v>257</v>
       </c>
       <c r="I51" s="6">
         <v>3</v>
       </c>
-      <c r="J51" s="8">
+      <c r="J51" s="24">
         <v>45580</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L51" s="25">
+        <v>228</v>
+      </c>
+      <c r="L51" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3745,33 +3737,33 @@
         <v>59</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E52" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G52" s="19" t="s">
+        <v>380</v>
+      </c>
+      <c r="H52" s="13" t="s">
         <v>258</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="G52" s="20" t="s">
-        <v>381</v>
-      </c>
-      <c r="H52" s="14" t="s">
-        <v>259</v>
       </c>
       <c r="I52" s="6">
         <v>3</v>
       </c>
-      <c r="J52" s="8">
+      <c r="J52" s="24">
         <v>45580</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L52" s="25">
+        <v>228</v>
+      </c>
+      <c r="L52" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3783,33 +3775,33 @@
         <v>79</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E53" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="G53" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="H53" s="13" t="s">
         <v>260</v>
-      </c>
-      <c r="F53" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G53" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="H53" s="14" t="s">
-        <v>261</v>
       </c>
       <c r="I53" s="6">
         <v>5</v>
       </c>
-      <c r="J53" s="8">
+      <c r="J53" s="24">
         <v>45580</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L53" s="25">
+        <v>228</v>
+      </c>
+      <c r="L53" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3821,33 +3813,33 @@
         <v>74</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E54" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="G54" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="H54" s="13" t="s">
         <v>262</v>
-      </c>
-      <c r="F54" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G54" s="20" t="s">
-        <v>383</v>
-      </c>
-      <c r="H54" s="14" t="s">
-        <v>263</v>
       </c>
       <c r="I54" s="6">
         <v>4</v>
       </c>
-      <c r="J54" s="8">
+      <c r="J54" s="24">
         <v>45580</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L54" s="25">
+        <v>228</v>
+      </c>
+      <c r="L54" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3859,33 +3851,33 @@
         <v>71</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E55" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G55" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="F55" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="G55" s="6" t="s">
+      <c r="H55" s="13" t="s">
         <v>265</v>
-      </c>
-      <c r="H55" s="14" t="s">
-        <v>266</v>
       </c>
       <c r="I55" s="6">
         <v>3</v>
       </c>
-      <c r="J55" s="8">
+      <c r="J55" s="24">
         <v>45580</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L55" s="25">
+        <v>228</v>
+      </c>
+      <c r="L55" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -3897,33 +3889,33 @@
         <v>64</v>
       </c>
       <c r="C56" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E56" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E56" s="14" t="s">
+      <c r="F56" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="F56" s="14" t="s">
+      <c r="G56" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="G56" s="6" t="s">
+      <c r="H56" s="13" t="s">
         <v>270</v>
-      </c>
-      <c r="H56" s="14" t="s">
-        <v>271</v>
       </c>
       <c r="I56" s="6">
         <v>2</v>
       </c>
-      <c r="J56" s="8">
+      <c r="J56" s="24">
         <v>45579</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L56" s="25">
+        <v>229</v>
+      </c>
+      <c r="L56" s="24">
         <v>45579</v>
       </c>
     </row>
@@ -3935,33 +3927,33 @@
         <v>56</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E57" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="G57" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="F57" s="16" t="s">
-        <v>269</v>
-      </c>
-      <c r="G57" s="6" t="s">
+      <c r="H57" s="13" t="s">
         <v>273</v>
-      </c>
-      <c r="H57" s="14" t="s">
-        <v>274</v>
       </c>
       <c r="I57" s="6">
         <v>2</v>
       </c>
-      <c r="J57" s="8">
+      <c r="J57" s="24">
         <v>45579</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L57" s="25">
+        <v>229</v>
+      </c>
+      <c r="L57" s="24">
         <v>45579</v>
       </c>
     </row>
@@ -3973,33 +3965,33 @@
         <v>72</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E58" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="G58" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="F58" s="16" t="s">
-        <v>269</v>
-      </c>
-      <c r="G58" s="6" t="s">
+      <c r="H58" s="13" t="s">
         <v>276</v>
-      </c>
-      <c r="H58" s="14" t="s">
-        <v>277</v>
       </c>
       <c r="I58" s="6">
         <v>1</v>
       </c>
-      <c r="J58" s="8">
+      <c r="J58" s="24">
         <v>45579</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L58" s="25">
+        <v>229</v>
+      </c>
+      <c r="L58" s="24">
         <v>45579</v>
       </c>
     </row>
@@ -4011,33 +4003,33 @@
         <v>52</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E59" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="G59" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="F59" s="16" t="s">
-        <v>269</v>
-      </c>
-      <c r="G59" s="6" t="s">
+      <c r="H59" s="13" t="s">
         <v>279</v>
-      </c>
-      <c r="H59" s="14" t="s">
-        <v>280</v>
       </c>
       <c r="I59" s="6">
         <v>1</v>
       </c>
-      <c r="J59" s="8">
+      <c r="J59" s="24">
         <v>45579</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L59" s="25">
+        <v>229</v>
+      </c>
+      <c r="L59" s="24">
         <v>45579</v>
       </c>
     </row>
@@ -4049,33 +4041,33 @@
         <v>46</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E60" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="F60" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="G60" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="F60" s="16" t="s">
-        <v>269</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="H60" s="23" t="s">
-        <v>384</v>
+      <c r="H60" s="22" t="s">
+        <v>383</v>
       </c>
       <c r="I60" s="6">
         <v>2</v>
       </c>
-      <c r="J60" s="8">
+      <c r="J60" s="24">
         <v>45579</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L60" s="25">
+        <v>229</v>
+      </c>
+      <c r="L60" s="24">
         <v>45579</v>
       </c>
     </row>
@@ -4087,33 +4079,33 @@
         <v>60</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E61" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="G61" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="F61" s="16" t="s">
-        <v>269</v>
-      </c>
-      <c r="G61" s="17" t="s">
+      <c r="H61" s="13" t="s">
         <v>284</v>
-      </c>
-      <c r="H61" s="14" t="s">
-        <v>285</v>
       </c>
       <c r="I61" s="6">
         <v>1</v>
       </c>
-      <c r="J61" s="8">
+      <c r="J61" s="24">
         <v>45579</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L61" s="25">
+        <v>229</v>
+      </c>
+      <c r="L61" s="24">
         <v>45579</v>
       </c>
     </row>
@@ -4125,33 +4117,33 @@
         <v>77</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E62" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="F62" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="G62" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="F62" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="G62" s="6" t="s">
+      <c r="H62" s="13" t="s">
         <v>287</v>
-      </c>
-      <c r="H62" s="14" t="s">
-        <v>288</v>
       </c>
       <c r="I62" s="6">
         <v>3</v>
       </c>
-      <c r="J62" s="8">
+      <c r="J62" s="24">
         <v>45579</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L62" s="25">
+        <v>229</v>
+      </c>
+      <c r="L62" s="24">
         <v>45579</v>
       </c>
     </row>
@@ -4163,33 +4155,33 @@
         <v>67</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E63" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="G63" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="F63" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="G63" s="6" t="s">
+      <c r="H63" s="13" t="s">
         <v>290</v>
-      </c>
-      <c r="H63" s="14" t="s">
-        <v>291</v>
       </c>
       <c r="I63" s="6">
         <v>1</v>
       </c>
-      <c r="J63" s="8">
+      <c r="J63" s="24">
         <v>45579</v>
       </c>
       <c r="K63" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L63" s="25">
+        <v>229</v>
+      </c>
+      <c r="L63" s="24">
         <v>45579</v>
       </c>
     </row>
@@ -4201,33 +4193,33 @@
         <v>76</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E64" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="G64" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="F64" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="G64" s="6" t="s">
+      <c r="H64" s="13" t="s">
         <v>293</v>
-      </c>
-      <c r="H64" s="14" t="s">
-        <v>294</v>
       </c>
       <c r="I64" s="6">
         <v>1</v>
       </c>
-      <c r="J64" s="8">
+      <c r="J64" s="24">
         <v>45579</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L64" s="25">
+        <v>229</v>
+      </c>
+      <c r="L64" s="24">
         <v>45579</v>
       </c>
     </row>
@@ -4239,33 +4231,33 @@
         <v>57</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E65" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="G65" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="F65" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="G65" s="6" t="s">
+      <c r="H65" s="13" t="s">
         <v>296</v>
-      </c>
-      <c r="H65" s="14" t="s">
-        <v>297</v>
       </c>
       <c r="I65" s="6">
         <v>1</v>
       </c>
-      <c r="J65" s="8">
+      <c r="J65" s="24">
         <v>45579</v>
       </c>
       <c r="K65" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L65" s="25">
+        <v>229</v>
+      </c>
+      <c r="L65" s="24">
         <v>45579</v>
       </c>
     </row>
@@ -4277,37 +4269,37 @@
         <v>58</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E66" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="F66" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="G66" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="F66" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="G66" s="6" t="s">
+      <c r="H66" s="13" t="s">
         <v>299</v>
-      </c>
-      <c r="H66" s="14" t="s">
-        <v>300</v>
       </c>
       <c r="I66" s="6">
         <v>5</v>
       </c>
-      <c r="J66" s="8">
+      <c r="J66" s="24">
         <v>45579</v>
       </c>
       <c r="K66" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L66" s="25">
+        <v>229</v>
+      </c>
+      <c r="L66" s="24">
         <v>45579</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" ht="30">
       <c r="A67" s="2" t="s">
         <v>45</v>
       </c>
@@ -4315,33 +4307,33 @@
         <v>62</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="E67" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="F67" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="G67" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="F67" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="G67" s="6" t="s">
+      <c r="H67" s="13" t="s">
         <v>302</v>
-      </c>
-      <c r="H67" s="14" t="s">
-        <v>303</v>
       </c>
       <c r="I67" s="6">
         <v>2</v>
       </c>
-      <c r="J67" s="8">
+      <c r="J67" s="24">
         <v>45579</v>
       </c>
       <c r="K67" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L67" s="25">
+        <v>229</v>
+      </c>
+      <c r="L67" s="24">
         <v>45579</v>
       </c>
     </row>
@@ -4353,17 +4345,17 @@
         <v>68</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
+        <v>303</v>
+      </c>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
       <c r="G68" s="6"/>
-      <c r="H68" s="14"/>
+      <c r="H68" s="13"/>
       <c r="I68" s="6"/>
-      <c r="J68" s="8"/>
+      <c r="J68" s="24"/>
       <c r="K68" s="6"/>
       <c r="L68" s="6"/>
     </row>
@@ -4375,17 +4367,17 @@
         <v>63</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
+        <v>303</v>
+      </c>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
       <c r="G69" s="6"/>
-      <c r="H69" s="14"/>
+      <c r="H69" s="13"/>
       <c r="I69" s="6"/>
-      <c r="J69" s="8"/>
+      <c r="J69" s="24"/>
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
     </row>
@@ -4397,17 +4389,17 @@
         <v>55</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
+        <v>303</v>
+      </c>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
       <c r="G70" s="6"/>
-      <c r="H70" s="14"/>
+      <c r="H70" s="13"/>
       <c r="I70" s="6"/>
-      <c r="J70" s="8"/>
+      <c r="J70" s="24"/>
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
     </row>
@@ -4419,33 +4411,33 @@
         <v>22</v>
       </c>
       <c r="C71" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E71" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="E71" s="14" t="s">
+      <c r="F71" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G71" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="F71" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="H71" s="24" t="s">
-        <v>385</v>
+      <c r="H71" s="23" t="s">
+        <v>384</v>
       </c>
       <c r="I71" s="6">
         <v>1</v>
       </c>
-      <c r="J71" s="8">
+      <c r="J71" s="24">
         <v>45580</v>
       </c>
       <c r="K71" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L71" s="25">
+        <v>228</v>
+      </c>
+      <c r="L71" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -4457,29 +4449,29 @@
         <v>9</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="E72" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="E72" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="F72" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="F72" s="14" t="s">
+      <c r="G72" s="18" t="s">
         <v>309</v>
       </c>
-      <c r="G72" s="19" t="s">
+      <c r="H72" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="H72" s="14" t="s">
-        <v>311</v>
-      </c>
       <c r="I72" s="6"/>
-      <c r="J72" s="8"/>
+      <c r="J72" s="24"/>
       <c r="K72" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L72" s="25">
+        <v>228</v>
+      </c>
+      <c r="L72" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -4491,29 +4483,29 @@
         <v>2</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="E73" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="E73" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="F73" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G73" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="F73" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="G73" s="6" t="s">
+      <c r="H73" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="H73" s="14" t="s">
-        <v>314</v>
-      </c>
       <c r="I73" s="6"/>
-      <c r="J73" s="8"/>
+      <c r="J73" s="24"/>
       <c r="K73" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L73" s="25">
+        <v>228</v>
+      </c>
+      <c r="L73" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -4525,29 +4517,29 @@
         <v>20</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E74" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="F74" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="G74" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="F74" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G74" s="6" t="s">
+      <c r="H74" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="H74" s="5" t="s">
-        <v>317</v>
-      </c>
       <c r="I74" s="6"/>
-      <c r="J74" s="8"/>
+      <c r="J74" s="24"/>
       <c r="K74" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L74" s="25">
+        <v>228</v>
+      </c>
+      <c r="L74" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -4559,17 +4551,17 @@
         <v>13</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E75" s="5"/>
-      <c r="F75" s="14"/>
+      <c r="F75" s="13"/>
       <c r="G75" s="6"/>
       <c r="H75" s="5"/>
       <c r="I75" s="6"/>
-      <c r="J75" s="8"/>
+      <c r="J75" s="24"/>
       <c r="K75" s="6"/>
       <c r="L75" s="6"/>
     </row>
@@ -4581,17 +4573,17 @@
         <v>16</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E76" s="5"/>
-      <c r="F76" s="14"/>
+      <c r="F76" s="13"/>
       <c r="G76" s="6"/>
       <c r="H76" s="5"/>
       <c r="I76" s="6"/>
-      <c r="J76" s="8"/>
+      <c r="J76" s="24"/>
       <c r="K76" s="6"/>
       <c r="L76" s="6"/>
     </row>
@@ -4603,17 +4595,17 @@
         <v>14</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E77" s="5"/>
-      <c r="F77" s="14"/>
+      <c r="F77" s="13"/>
       <c r="G77" s="6"/>
       <c r="H77" s="5"/>
       <c r="I77" s="6"/>
-      <c r="J77" s="8"/>
+      <c r="J77" s="24"/>
       <c r="K77" s="6"/>
       <c r="L77" s="6"/>
     </row>
@@ -4625,29 +4617,29 @@
         <v>4</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E78" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="F78" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="F78" s="14" t="s">
+      <c r="G78" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="G78" s="6" t="s">
+      <c r="H78" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="H78" s="5" t="s">
-        <v>321</v>
-      </c>
       <c r="I78" s="6"/>
-      <c r="J78" s="8"/>
+      <c r="J78" s="24"/>
       <c r="K78" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L78" s="25">
+        <v>228</v>
+      </c>
+      <c r="L78" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -4659,21 +4651,21 @@
         <v>18</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
       <c r="G79" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="H79" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="H79" s="5" t="s">
-        <v>323</v>
-      </c>
       <c r="I79" s="6"/>
-      <c r="J79" s="8"/>
+      <c r="J79" s="24"/>
       <c r="K79" s="6"/>
       <c r="L79" s="6"/>
     </row>
@@ -4685,33 +4677,33 @@
         <v>5</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E80" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G80" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="F80" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G80" s="6" t="s">
+      <c r="H80" s="5" t="s">
         <v>325</v>
-      </c>
-      <c r="H80" s="5" t="s">
-        <v>326</v>
       </c>
       <c r="I80" s="6">
         <v>1</v>
       </c>
-      <c r="J80" s="8">
+      <c r="J80" s="24">
         <v>45582</v>
       </c>
       <c r="K80" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L80" s="25">
+        <v>228</v>
+      </c>
+      <c r="L80" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -4723,29 +4715,29 @@
         <v>99</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E81" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G81" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="F81" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G81" s="6" t="s">
+      <c r="H81" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="H81" s="5" t="s">
-        <v>329</v>
-      </c>
       <c r="I81" s="6"/>
-      <c r="J81" s="8"/>
+      <c r="J81" s="24"/>
       <c r="K81" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L81" s="25">
+        <v>228</v>
+      </c>
+      <c r="L81" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -4757,33 +4749,33 @@
         <v>8</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>118</v>
       </c>
       <c r="G82" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="H82" s="5" t="s">
         <v>331</v>
-      </c>
-      <c r="H82" s="5" t="s">
-        <v>332</v>
       </c>
       <c r="I82" s="6">
         <v>1</v>
       </c>
-      <c r="J82" s="8">
+      <c r="J82" s="24">
         <v>45574</v>
       </c>
       <c r="K82" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L82" s="25">
+        <v>229</v>
+      </c>
+      <c r="L82" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -4795,17 +4787,17 @@
         <v>6</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
       <c r="G83" s="6"/>
       <c r="H83" s="5"/>
       <c r="I83" s="6"/>
-      <c r="J83" s="8"/>
+      <c r="J83" s="24"/>
       <c r="K83" s="6"/>
       <c r="L83" s="6"/>
     </row>
@@ -4817,29 +4809,29 @@
         <v>1</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E84" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G84" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="F84" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G84" s="6" t="s">
+      <c r="H84" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="H84" s="5" t="s">
-        <v>335</v>
-      </c>
       <c r="I84" s="6"/>
-      <c r="J84" s="8"/>
+      <c r="J84" s="24"/>
       <c r="K84" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L84" s="25">
+        <v>228</v>
+      </c>
+      <c r="L84" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -4851,17 +4843,17 @@
         <v>17</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
       <c r="G85" s="6"/>
       <c r="H85" s="5"/>
       <c r="I85" s="6"/>
-      <c r="J85" s="8"/>
+      <c r="J85" s="24"/>
       <c r="K85" s="6"/>
       <c r="L85" s="6"/>
     </row>
@@ -4873,29 +4865,29 @@
         <v>23</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E86" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G86" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="F86" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G86" s="6" t="s">
+      <c r="H86" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="H86" s="5" t="s">
-        <v>338</v>
-      </c>
       <c r="I86" s="6"/>
-      <c r="J86" s="8"/>
+      <c r="J86" s="24"/>
       <c r="K86" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L86" s="25">
+        <v>228</v>
+      </c>
+      <c r="L86" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -4907,29 +4899,29 @@
         <v>3</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>118</v>
       </c>
       <c r="G87" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="H87" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="H87" s="5" t="s">
-        <v>341</v>
-      </c>
       <c r="I87" s="6"/>
-      <c r="J87" s="8"/>
+      <c r="J87" s="24"/>
       <c r="K87" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L87" s="25">
+        <v>228</v>
+      </c>
+      <c r="L87" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -4941,17 +4933,17 @@
         <v>7</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
       <c r="G88" s="6"/>
       <c r="H88" s="5"/>
       <c r="I88" s="6"/>
-      <c r="J88" s="8"/>
+      <c r="J88" s="24"/>
       <c r="K88" s="6"/>
       <c r="L88" s="6"/>
     </row>
@@ -4963,17 +4955,17 @@
         <v>12</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
       <c r="G89" s="6"/>
       <c r="H89" s="5"/>
       <c r="I89" s="6"/>
-      <c r="J89" s="8"/>
+      <c r="J89" s="24"/>
       <c r="K89" s="6"/>
       <c r="L89" s="6"/>
     </row>
@@ -4985,33 +4977,33 @@
         <v>15</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E90" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="F90" s="5" t="s">
+      <c r="G90" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="G90" s="6" t="s">
+      <c r="H90" s="5" t="s">
         <v>344</v>
-      </c>
-      <c r="H90" s="5" t="s">
-        <v>345</v>
       </c>
       <c r="I90" s="6">
         <v>1</v>
       </c>
-      <c r="J90" s="8">
+      <c r="J90" s="24">
         <v>45580</v>
       </c>
       <c r="K90" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L90" s="25">
+        <v>229</v>
+      </c>
+      <c r="L90" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -5023,29 +5015,29 @@
         <v>10</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F91" s="5" t="s">
         <v>118</v>
       </c>
       <c r="G91" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="H91" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="H91" s="5" t="s">
-        <v>348</v>
-      </c>
       <c r="I91" s="6"/>
-      <c r="J91" s="8"/>
+      <c r="J91" s="24"/>
       <c r="K91" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L91" s="25">
+        <v>228</v>
+      </c>
+      <c r="L91" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -5057,29 +5049,29 @@
         <v>44</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F92" s="5" t="s">
         <v>118</v>
       </c>
       <c r="G92" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="H92" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="H92" s="5" t="s">
-        <v>351</v>
-      </c>
       <c r="I92" s="6"/>
-      <c r="J92" s="8"/>
+      <c r="J92" s="24"/>
       <c r="K92" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L92" s="25">
+        <v>228</v>
+      </c>
+      <c r="L92" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -5091,29 +5083,29 @@
         <v>19</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E93" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G93" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="F93" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G93" s="6" t="s">
+      <c r="H93" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="H93" s="5" t="s">
-        <v>354</v>
-      </c>
       <c r="I93" s="6"/>
-      <c r="J93" s="8"/>
+      <c r="J93" s="24"/>
       <c r="K93" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L93" s="25">
+        <v>228</v>
+      </c>
+      <c r="L93" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -5125,29 +5117,29 @@
         <v>21</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E94" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G94" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="H94" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="F94" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G94" s="20" t="s">
-        <v>387</v>
-      </c>
-      <c r="H94" s="5" t="s">
-        <v>356</v>
-      </c>
       <c r="I94" s="6"/>
-      <c r="J94" s="8"/>
+      <c r="J94" s="24"/>
       <c r="K94" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L94" s="25">
+        <v>228</v>
+      </c>
+      <c r="L94" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -5159,29 +5151,29 @@
         <v>98</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E95" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G95" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="F95" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G95" s="6" t="s">
+      <c r="H95" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="H95" s="5" t="s">
-        <v>359</v>
-      </c>
       <c r="I95" s="6"/>
-      <c r="J95" s="8"/>
+      <c r="J95" s="24"/>
       <c r="K95" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L95" s="25">
+        <v>228</v>
+      </c>
+      <c r="L95" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -5193,29 +5185,29 @@
         <v>50</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E96" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G96" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="F96" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G96" s="6" t="s">
+      <c r="H96" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="H96" s="5" t="s">
-        <v>362</v>
-      </c>
       <c r="I96" s="6"/>
-      <c r="J96" s="8"/>
+      <c r="J96" s="24"/>
       <c r="K96" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="L96" s="25">
+        <v>228</v>
+      </c>
+      <c r="L96" s="24">
         <v>45566</v>
       </c>
     </row>
@@ -5227,33 +5219,33 @@
         <v>11</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F97" s="5" t="s">
         <v>118</v>
       </c>
       <c r="G97" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="H97" s="5" t="s">
         <v>364</v>
-      </c>
-      <c r="H97" s="5" t="s">
-        <v>365</v>
       </c>
       <c r="I97" s="6">
         <v>1</v>
       </c>
-      <c r="J97" s="8">
+      <c r="J97" s="24">
         <v>45574</v>
       </c>
       <c r="K97" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="L97" s="25">
+        <v>229</v>
+      </c>
+      <c r="L97" s="24">
         <v>45566</v>
       </c>
     </row>

</xml_diff>